<commit_message>
added updated bug report
</commit_message>
<xml_diff>
--- a/doc/bug_report.xlsx
+++ b/doc/bug_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>#</t>
   </si>
@@ -117,9 +117,6 @@
     <t xml:space="preserve">Luke </t>
   </si>
   <si>
-    <t>in-progress</t>
-  </si>
-  <si>
     <t>Logan</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>Press one key (left or right) going into a side wall and one key either up or down. Drag player along walls for at most ten seconds and the player will get stuck, even when keys are released.</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>Enemies sometimes go into walls after knockback</t>
   </si>
   <si>
@@ -201,6 +195,21 @@
   </si>
   <si>
     <t>Walk towards a 1x3 furniture object that is against the wall on the y axis and x axis on at least one side for both.</t>
+  </si>
+  <si>
+    <t>won't fix</t>
+  </si>
+  <si>
+    <t>Screen doesn't darken immediately coming into level from menu</t>
+  </si>
+  <si>
+    <t>Screen should darken immediately when entering level from menu screen, and only be fully light (no diffused lighting model) when all enemies are killed</t>
+  </si>
+  <si>
+    <t>Screen takes a few seconds, and then adds illumination model</t>
+  </si>
+  <si>
+    <t>Enter a level other than level 1 from the menu screen.</t>
   </si>
 </sst>
 </file>
@@ -948,22 +957,22 @@
         <v>11</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="H6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="J6" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7">
@@ -983,19 +992,19 @@
         <v>12</v>
       </c>
       <c r="F7" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="H7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="I7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="J7" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8">
@@ -1006,7 +1015,7 @@
         <v>45599.0</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>22</v>
@@ -1015,19 +1024,19 @@
         <v>12</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="J8" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -1038,28 +1047,28 @@
         <v>45599.0</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="13" t="s">
-        <v>33</v>
+      <c r="G9" s="15" t="s">
+        <v>46</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="H9" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="I9" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="J9" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10">
@@ -1070,28 +1079,28 @@
         <v>45614.0</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="I10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="J10" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -1102,41 +1111,61 @@
         <v>45614.0</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="J11" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="16" t="s">
+    </row>
+    <row r="12">
+      <c r="A12" s="4">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="5">
+        <v>45628.0</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="F12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+      <c r="H12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="11"/>

</xml_diff>